<commit_message>
Agregar Ontología y anexos
La ontología estaba en otro GitHub , se incluyó aquí.
</commit_message>
<xml_diff>
--- a/FocusGroup/Resultados en tabla.xlsx
+++ b/FocusGroup/Resultados en tabla.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d2a2aabdc201144/Documentos2016/Unicomfacauca/2019-II/Investigación/ProyectoUEES/Informe Final/Anexos/Anexo 5/FocusGroup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d2a2aabdc201144/Documentos2016/Unicomfacauca/2020-I/Investigación/Artículos/02-FameSIS/FrameD-SIS/FrameD-SIS/FocusGroup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_2379E3D40F958F05A1E0510255E39198610B5F71" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E17E3CA1-6AEB-450F-8FAD-D20848B4B7C8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_2379E3D40F958F05A1E0510255E39198610B5F71" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2A2681C9-8CC5-4D34-AB24-61C7FDEF9D47}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="gráfica" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <r>
       <t> </t>
@@ -117,12 +118,6 @@
     <t>¿Considera usted que hay aspectos limitantes en el framework propuesto?</t>
   </si>
   <si>
-    <t>promedio</t>
-  </si>
-  <si>
-    <t>Ontología</t>
-  </si>
-  <si>
     <t>Framework</t>
   </si>
   <si>
@@ -130,6 +125,9 @@
   </si>
   <si>
     <t>Aspecto Negativo</t>
+  </si>
+  <si>
+    <t>Preguntas extras</t>
   </si>
 </sst>
 </file>
@@ -261,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -277,9 +275,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -323,6 +318,1178 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-US"/>
+              <a:t>Resultados del</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-US" baseline="0"/>
+              <a:t> Grupo Focal </a:t>
+            </a:r>
+            <a:endParaRPr lang="es-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aspecto Positivo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>La ontología presenta la información suficiente para definir los requisitos necesarios para el desarrollo de sistemas para SSR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>La ontología presentada permite identificar los términos y lenguaje adecuado en SSR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>La ontología propuesta es de fácil uso para los desarrolladores de sistemas para SSR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Las fuentes de datos que proporciona la ontología son suficientes para definir los modelos de información</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>La guía de uso del framework es apropiada para ser utilizadas por desarrolladores de sistemas para SSR</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>El framework propuesto permite solucionar los problemas identificados en el sector</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>El diagrama presentado describe de forma clara el framework propuesto </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>La dimensión de salud sexual y reproductiva es relevante para una versión inicial del framework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.6428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92307692307692313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90909090909090906</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-52BE-4D52-A04F-95F6A9D80781}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aspecto Negativo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>La ontología presenta la información suficiente para definir los requisitos necesarios para el desarrollo de sistemas para SSR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>La ontología presentada permite identificar los términos y lenguaje adecuado en SSR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>La ontología propuesta es de fácil uso para los desarrolladores de sistemas para SSR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Las fuentes de datos que proporciona la ontología son suficientes para definir los modelos de información</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>La guía de uso del framework es apropiada para ser utilizadas por desarrolladores de sistemas para SSR</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>El framework propuesto permite solucionar los problemas identificados en el sector</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>El diagrama presentado describe de forma clara el framework propuesto </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>La dimensión de salud sexual y reproductiva es relevante para una versión inicial del framework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$J$2:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.35714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6923076923076927E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-52BE-4D52-A04F-95F6A9D80781}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:overlap val="100"/>
+        <c:axId val="495249600"/>
+        <c:axId val="495242712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="495249600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495242712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="495242712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495249600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{030C8AD3-E0B0-41FD-A1BA-EB3B6CE227F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -588,20 +1755,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" activeCellId="1" sqref="B1:B9 I1:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="55.109375" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="12" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -615,17 +1783,21 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>24</v>
+      <c r="F1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -639,35 +1811,36 @@
         <v>5</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <f>C2</f>
         <v>9</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <f>D2+E2</f>
         <v>5</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="11"/>
+      <c r="I2" s="7">
         <f>F2/(14-E2)</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="I2" s="8">
+      <c r="J2" s="7">
         <f>D2/(C2+D2)</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="10">
-        <f>AVERAGE(H2:H5)</f>
-        <v>0.8392857142857143</v>
-      </c>
-      <c r="L2" s="10">
-        <f>AVERAGE(I2:I5)</f>
-        <v>0.1607142857142857</v>
+      <c r="K2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="9">
+        <f>AVERAGE(I2:I11)</f>
+        <v>0.71893106893106895</v>
+      </c>
+      <c r="M2" s="9">
+        <f>AVERAGE(J2:J11)</f>
+        <v>8.1068931068931066E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -681,35 +1854,25 @@
       <c r="E3" s="6">
         <v>2</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <f>C3</f>
         <v>12</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <f>D3+E3</f>
         <v>2</v>
       </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H12" si="0">F3/(14-E3)</f>
+      <c r="H3" s="11"/>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I11" si="0">F3/(14-E3)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="8">
-        <f t="shared" ref="I3:I11" si="1">D3/(C3+D3)</f>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J11" si="1">D3/(C3+D3)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="10">
-        <f>AVERAGE(H2:H11)</f>
-        <v>0.71893106893106895</v>
-      </c>
-      <c r="L3" s="10">
-        <f>AVERAGE(I2:I11)</f>
-        <v>8.1068931068931066E-2</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -723,24 +1886,25 @@
       <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F4" s="12">
-        <f t="shared" ref="F4:F11" si="2">C4</f>
+      <c r="F4" s="11">
+        <f t="shared" ref="F4:F9" si="2">C4</f>
         <v>11</v>
       </c>
-      <c r="G4" s="12">
-        <f t="shared" ref="G4:G11" si="3">D4+E4</f>
+      <c r="G4" s="11">
+        <f t="shared" ref="G4:G9" si="3">D4+E4</f>
         <v>3</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="11"/>
+      <c r="I4" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J4" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -756,24 +1920,25 @@
       <c r="E5" s="6">
         <v>7</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="11"/>
+      <c r="I5" s="7">
         <f t="shared" si="0"/>
         <v>0.7142857142857143</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J5" s="7">
         <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -789,24 +1954,25 @@
       <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <f>C6</f>
         <v>12</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <f>D6</f>
         <v>1</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="11"/>
+      <c r="I6" s="7">
         <f t="shared" si="0"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J6" s="7">
         <f t="shared" si="1"/>
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -822,24 +1988,25 @@
       <c r="E7" s="6">
         <v>3</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="11"/>
+      <c r="I7" s="7">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="7">
         <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -853,24 +2020,25 @@
       <c r="E8" s="6">
         <v>2</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="11"/>
+      <c r="I8" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -884,90 +2052,114 @@
       <c r="E9" s="6">
         <v>2</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="11"/>
+      <c r="I9" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9" s="8">
+      <c r="J9" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>7</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14">
         <v>7</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <f>D10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="15">
         <f>C10</f>
         <v>7</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="15"/>
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="17">
+      <c r="J10" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>7</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14">
         <v>7</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <f>D11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <f>C11</f>
         <v>7</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="15"/>
+      <c r="I11" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="17">
+      <c r="J11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H12" s="8"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74357F38-1FA6-4521-978C-E875E803CB75}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>